<commit_message>
start topologicalSort & segmentTree
</commit_message>
<xml_diff>
--- a/src/main/java/leetcode/com/tag/Number_List.xlsx
+++ b/src/main/java/leetcode/com/tag/Number_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="34780" yWindow="1040" windowWidth="28800" windowHeight="17040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -168,6 +168,16 @@
     <t>树的三种非递归遍历方式需要再重温下，这道题就是非递归遍历的变种</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>1. dp配合dfs解决问题，看上去很难，但是如果已知dfs的递归解法，再配合dp的概念就没那么难理解啦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.buildTree的时候，要用到数组的递归循环呢，要搞清楚哦
+2.update value的时候，要注意更新
+3.sum的时候，下标的判断和方法参数中的下标传递方式也要注意，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -308,7 +318,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -330,6 +340,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -691,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F700"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F174" sqref="F174"/>
+    <sheetView tabSelected="1" topLeftCell="A306" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E313" sqref="E313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -713,7 +726,7 @@
       </c>
       <c r="C1" s="8">
         <f>COUNTIF(C2:C700,"&gt;=0")</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -4305,16 +4318,22 @@
       <c r="E307" s="2"/>
       <c r="F307" s="2"/>
     </row>
-    <row r="308" spans="1:6">
+    <row r="308" spans="1:6" ht="45">
       <c r="A308" s="5">
         <f t="shared" si="4"/>
         <v>307</v>
       </c>
-      <c r="B308" s="2"/>
-      <c r="C308" s="9"/>
+      <c r="B308" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C308" s="9">
+        <v>1</v>
+      </c>
       <c r="D308" s="2"/>
       <c r="E308" s="2"/>
-      <c r="F308" s="2"/>
+      <c r="F308" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="309" spans="1:6">
       <c r="A309" s="5">
@@ -4551,16 +4570,22 @@
       <c r="E329" s="2"/>
       <c r="F329" s="2"/>
     </row>
-    <row r="330" spans="1:6">
+    <row r="330" spans="1:6" ht="30">
       <c r="A330" s="5">
         <f t="shared" si="5"/>
         <v>329</v>
       </c>
-      <c r="B330" s="2"/>
-      <c r="C330" s="9"/>
+      <c r="B330" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C330" s="9">
+        <v>1</v>
+      </c>
       <c r="D330" s="2"/>
       <c r="E330" s="2"/>
-      <c r="F330" s="2"/>
+      <c r="F330" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="331" spans="1:6">
       <c r="A331" s="5">

</xml_diff>